<commit_message>
Start with grade3 conduct
</commit_message>
<xml_diff>
--- a/EX_conductivity_data.xlsx
+++ b/EX_conductivity_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,16 +15,13 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1277,10 +1274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G17"/>
+  <dimension ref="A2:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,14 +1314,14 @@
         <v>735</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B6" si="0">A3/1.1</f>
+        <f>A3/1.1</f>
         <v>668.18181818181813</v>
       </c>
       <c r="C3">
         <v>2077</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D5" si="1">1000000/B3</f>
+        <f>1000000/B3</f>
         <v>1496.5986394557824</v>
       </c>
       <c r="E3">
@@ -1337,14 +1334,14 @@
         <v>1640</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
+        <f>A4/1.1</f>
         <v>1490.9090909090908</v>
       </c>
       <c r="C4">
         <v>4636</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
+        <f>1000000/B4</f>
         <v>670.73170731707319</v>
       </c>
     </row>
@@ -1353,14 +1350,14 @@
         <v>14230</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f>A5/1.1</f>
         <v>12936.363636363636</v>
       </c>
       <c r="C5">
         <v>42300</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
+        <f>1000000/B5</f>
         <v>77.301475755446248</v>
       </c>
     </row>
@@ -1369,7 +1366,7 @@
         <v>18200</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f>A6/1.1</f>
         <v>16545.454545454544</v>
       </c>
       <c r="C6">
@@ -1377,7 +1374,7 @@
         <v>59545.684277897497</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6" si="2">1000000/A6</f>
+        <f>1000000/A6</f>
         <v>54.945054945054942</v>
       </c>
     </row>
@@ -1413,8 +1410,8 @@
         <v>281.60000000000002</v>
       </c>
       <c r="D13">
-        <f>INTERCEPT(A13:A14,B13:B14)</f>
-        <v>5.7149467310273394</v>
+        <f>INTERCEPT(B13:B14,A13:A14)</f>
+        <v>-25.961064425770928</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1422,17 +1419,79 @@
         <v>8746</v>
       </c>
       <c r="B14">
-        <v>14286</v>
+        <v>15086</v>
       </c>
       <c r="D14">
-        <f>SLOPE(A13:A14,B13:B14)</f>
-        <v>0.61180771757447661</v>
+        <f>SLOPE(B13:B14,A13:A14)</f>
+        <v>1.7278711484593838</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17">
-        <f>8746*0.612 + 6</f>
-        <v>5358.5519999999997</v>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D15" t="e">
+        <f>INTERCEPT(B15:B16,A15:A16)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D16" t="e">
+        <f>SLOPE(B15:B16,A15:A16)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>141</v>
+      </c>
+      <c r="B18">
+        <v>225</v>
+      </c>
+      <c r="D18">
+        <f>INTERCEPT(B18:B19,A18:A19)</f>
+        <v>-49.71005853024144</v>
+      </c>
+      <c r="G18">
+        <f>1/0.055</f>
+        <v>18.181818181818183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>9367</v>
+      </c>
+      <c r="B19">
+        <v>18200</v>
+      </c>
+      <c r="D19">
+        <f>SLOPE(B18:B19,A18:A19)</f>
+        <v>1.9482982874485151</v>
+      </c>
+      <c r="G19">
+        <f>1/4.45</f>
+        <v>0.2247191011235955</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>68</v>
+      </c>
+      <c r="B21">
+        <v>25</v>
+      </c>
+      <c r="D21">
+        <f>INTERCEPT(B21:B22,A21:A22)</f>
+        <v>-2.0612244897959044</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2518</v>
+      </c>
+      <c r="B22">
+        <v>1000</v>
+      </c>
+      <c r="D22">
+        <f>SLOPE(B21:B22,A21:A22)</f>
+        <v>0.39795918367346939</v>
       </c>
     </row>
   </sheetData>

</xml_diff>